<commit_message>
Fixed create flight method to properly add a flight to table
</commit_message>
<xml_diff>
--- a/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
+++ b/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxvia\Documents\GitHub\EECS-3550-Team-2\SWE Project\SWE Project\bin\Debug\net6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A9B0CB-9419-4B7C-B700-FF08A095B9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B7EC7B-9350-4A29-8EF5-AB76E320625B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>UserID</t>
   </si>
@@ -127,6 +127,30 @@
   </si>
   <si>
     <t>Booked Capacity</t>
+  </si>
+  <si>
+    <t>FlightId</t>
+  </si>
+  <si>
+    <t>DepartingFrom</t>
+  </si>
+  <si>
+    <t>ArrivingAt</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>houston airport</t>
+  </si>
+  <si>
+    <t>Nebraska airport</t>
+  </si>
+  <si>
+    <t>4/6/2023</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -174,7 +198,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -317,16 +361,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:J3" totalsRowShown="0">
   <autoFilter ref="A1:J3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="UserID" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Password" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FirstName" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="LastName" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Address" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Phone" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Age" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Wallet" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardPoints" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CardInfo" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="UserID" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Password" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FirstName" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="LastName" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Address" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Phone" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Age" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Wallet" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardPoints" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CardInfo" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -336,13 +380,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:G3" totalsRowShown="0">
   <autoFilter ref="A1:G3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CustID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="FlightID" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Date" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Status" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="From" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Destination" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Points Used" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CustID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="FlightID" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Date" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Status" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="From" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Destination" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Points Used" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -352,10 +396,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="EmpID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Password" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FirstName" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="LastName" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="EmpID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Password" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FirstName" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="LastName" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -365,10 +409,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="FlightManifest" displayName="FlightManifest" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="FlightID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Income" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Total Capacity" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Booked Capacity" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="FlightID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Income" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Total Capacity" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Booked Capacity" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="FlightId" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DepartingFrom" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ArrivingAt" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="DateTime" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -930,12 +987,49 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EA6902-D596-40FD-BE4B-863FCFD1EB94}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="5" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New Branch + Load Engineer methods
- Finished Edit Flight and Delete Flight methods (The parts that don't interact with customers)
</commit_message>
<xml_diff>
--- a/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
+++ b/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxvia\Documents\GitHub\EECS-3550-Team-2\SWE Project\SWE Project\bin\Debug\net6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B7EC7B-9350-4A29-8EF5-AB76E320625B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B282078-1BDA-40F7-814C-0C544FBC1444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>UserID</t>
   </si>
@@ -141,16 +141,25 @@
     <t>DateTime</t>
   </si>
   <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>nashville</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>4/7/2023 5:50 PM</t>
+  </si>
+  <si>
+    <t>456</t>
+  </si>
+  <si>
+    <t>Nebraska airport</t>
+  </si>
+  <si>
     <t>houston airport</t>
-  </si>
-  <si>
-    <t>Nebraska airport</t>
-  </si>
-  <si>
-    <t>4/6/2023</t>
-  </si>
-  <si>
-    <t>123</t>
   </si>
 </sst>
 </file>
@@ -172,15 +181,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -188,37 +203,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <font>
         <color theme="1"/>
@@ -361,16 +400,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:J3" totalsRowShown="0">
   <autoFilter ref="A1:J3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="UserID" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Password" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FirstName" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="LastName" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Address" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Phone" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Age" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Wallet" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardPoints" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CardInfo" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="UserID" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Password" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FirstName" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="LastName" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Address" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Phone" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Age" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Wallet" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="RewardPoints" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="CardInfo" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -380,13 +419,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table4" displayName="Table4" ref="A1:G3" totalsRowShown="0">
   <autoFilter ref="A1:G3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CustID" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="FlightID" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Date" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Status" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="From" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Destination" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Points Used" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CustID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="FlightID" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Date" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Status" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="From" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Destination" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Points Used" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -396,10 +435,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="EmpID" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Password" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FirstName" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="LastName" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="EmpID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Password" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FirstName" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="LastName" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -409,23 +448,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="FlightManifest" displayName="FlightManifest" ref="A1:D2" totalsRowShown="0">
   <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="FlightID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Income" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Total Capacity" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Booked Capacity" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="FlightID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Income" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Total Capacity" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Booked Capacity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A1:D2" totalsRowShown="0">
-  <autoFilter ref="A1:D2" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table6" displayName="Table6" ref="A1:D3" totalsRowShown="0">
+  <autoFilter ref="A1:D3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="FlightId" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DepartingFrom" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ArrivingAt" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="DateTime" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="FlightId"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DepartingFrom"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="ArrivingAt"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="DateTime"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -987,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EA6902-D596-40FD-BE4B-863FCFD1EB94}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +1037,7 @@
     <col min="1" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1012,19 +1051,43 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished Accountant income of one flight
- Changed passenger list in flight objects to be a list of customers
</commit_message>
<xml_diff>
--- a/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
+++ b/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxvia\Documents\GitHub\EECS-3550-Team-2\SWE Project\SWE Project\bin\Debug\net6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1968B15-0117-4ABC-A7F3-5CB10F667900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC8274B-96E7-496D-9D62-2F887CF155E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="2820" windowWidth="14220" windowHeight="11385" firstSheet="1" activeTab="4" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
   </bookViews>
   <sheets>
     <sheet name="CustList" sheetId="1" r:id="rId1"/>
@@ -1068,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F89F44-A481-4375-B1EC-C94DE9571F7E}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EA6902-D596-40FD-BE4B-863FCFD1EB94}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Fixed Password for login
</commit_message>
<xml_diff>
--- a/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
+++ b/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxvia\Documents\GitHub\EECS-3550-Team-2\SWE Project\SWE Project\bin\Debug\net6.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8f136795524a28e/Documents/GitHub/EECS-3550-Team-2/SWE Project/SWE Project/bin/Debug/net6.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934914E8-EC74-4613-BE99-842BB9B53940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{934914E8-EC74-4613-BE99-842BB9B53940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB59C54-DEC7-4846-BA85-3D6449242FC4}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="5" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
+    <x:workbookView xWindow="1815" yWindow="1815" windowWidth="15375" windowHeight="7875" firstSheet="0" activeTab="0" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="CustList" sheetId="1" r:id="rId1"/>
@@ -87,6 +87,60 @@
   </x:si>
   <x:si>
     <x:t>321 Ren Rd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2E9B40BC8C1D34338C899A843ABAAE2D</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Wamer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Isaac</x:t>
+  </x:si>
+  <x:si>
+    <x:t>123 Dunk</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jajajaja</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>051A9911DE7B5BBC610B76F4EDA834A0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>f</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2DB95E8E1A9267B7A1188556B2013B33</x:t>
+  </x:si>
+  <x:si>
+    <x:t>l</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System.Byte[]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>p</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System.Char[]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>i</x:t>
+  </x:si>
+  <x:si>
+    <x:t>w</x:t>
+  </x:si>
+  <x:si>
+    <x:t>_x001F_@���$_x0016_�u	y�l�����Ҏ_x0018_3]�Z�T�V_x000E__x000F_S_x0002_�_x000C_e+��V_x0002_R�^t!_x0005_F�i��Ό_x0012_�Ǖ{&amp;R��u</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aa</x:t>
   </x:si>
   <x:si>
     <x:t>CustID</x:t>
@@ -379,7 +433,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="22">
+  <x:cellXfs count="15">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -388,15 +442,10 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <x:xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <x:xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <x:xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <x:alignment vertical="center"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -409,14 +458,6 @@
     </x:xf>
     <x:xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -433,12 +474,12 @@
     </x:dxf>
     <x:dxf>
       <x:font>
-        <x:b/>
         <x:sz val="10"/>
       </x:font>
     </x:dxf>
     <x:dxf>
       <x:font>
+        <x:b/>
         <x:sz val="10"/>
       </x:font>
     </x:dxf>
@@ -453,6 +494,10 @@
     </x:ext>
   </x:extLst>
 </x:styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,44 +520,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="SaltLakeCity" displayName="SaltLakeCity" ref="M1:N11" totalsRowShown="0">
-  <x:autoFilter ref="M1:N11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Detroit" displayName="Detroit" ref="S1:T11" totalsRowShown="0">
+  <x:autoFilter ref="S1:T11"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="City"/>
+    <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Nashville" displayName="Nashville" ref="A1:B11" totalsRowShown="0">
+  <x:autoFilter ref="A1:B11"/>
+  <x:tableColumns count="2">
+    <x:tableColumn id="1" name="City" dataDxfId="1"/>
     <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Miami" displayName="Miami" ref="P1:Q11" totalsRowShown="0">
-  <x:autoFilter ref="P1:Q11"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="LosAngeles" displayName="LosAngeles" ref="G1:H11" totalsRowShown="0">
+  <x:autoFilter ref="G1:H11"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="City"/>
-    <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
+    <x:tableColumn id="2" name="Distance"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Detroit" displayName="Detroit" ref="S1:T11" totalsRowShown="0">
-  <x:autoFilter ref="S1:T11"/>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="WashingtonDc" displayName="WashingtonDc" ref="AE1:AF11" totalsRowShown="0">
+  <x:autoFilter ref="AE1:AF11"/>
   <x:tableColumns count="2">
-    <x:tableColumn id="1" name="City"/>
-    <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Atlanta" displayName="Atlanta" ref="V1:W11" totalsRowShown="0">
-  <x:autoFilter ref="V1:W11"/>
-  <x:tableColumns count="2">
-    <x:tableColumn id="1" name="City"/>
-    <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
+    <x:tableColumn id="1" name="City" dataDxfId="1"/>
+    <x:tableColumn id="2" name="Distance"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -523,29 +568,29 @@
   <x:autoFilter ref="Y1:Z11"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="City"/>
-    <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
+    <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="LasVegas" displayName="LasVegas" ref="AB1:AC11" totalsRowShown="0">
-  <x:autoFilter ref="AB1:AC11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Miami" displayName="Miami" ref="P1:Q11" totalsRowShown="0">
+  <x:autoFilter ref="P1:Q11"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="City"/>
-    <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
+    <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="WashingtonDc" displayName="WashingtonDc" ref="AE1:AF11" totalsRowShown="0">
-  <x:autoFilter ref="AE1:AF11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="NewYorkCity" displayName="NewYorkCity" ref="J1:K11" totalsRowShown="0">
+  <x:autoFilter ref="J1:K11"/>
   <x:tableColumns count="2">
-    <x:tableColumn id="1" name="City" dataDxfId="2"/>
-    <x:tableColumn id="2" name="Distance"/>
+    <x:tableColumn id="1" name="City"/>
+    <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -607,10 +652,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Nashville" displayName="Nashville" ref="A1:B11" totalsRowShown="0">
-  <x:autoFilter ref="A1:B11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="LasVegas" displayName="LasVegas" ref="AB1:AC11" totalsRowShown="0">
+  <x:autoFilter ref="AB1:AC11"/>
   <x:tableColumns count="2">
-    <x:tableColumn id="1" name="City" dataDxfId="2"/>
+    <x:tableColumn id="1" name="City"/>
     <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -621,30 +666,30 @@
 <x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Cleveland" displayName="Cleveland" ref="D1:E11" totalsRowShown="0">
   <x:autoFilter ref="D1:E11"/>
   <x:tableColumns count="2">
-    <x:tableColumn id="1" name="City" dataDxfId="2"/>
-    <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
+    <x:tableColumn id="1" name="City" dataDxfId="1"/>
+    <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="LosAngeles" displayName="LosAngeles" ref="G1:H11" totalsRowShown="0">
-  <x:autoFilter ref="G1:H11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="SaltLakeCity" displayName="SaltLakeCity" ref="M1:N11" totalsRowShown="0">
+  <x:autoFilter ref="M1:N11"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="City"/>
-    <x:tableColumn id="2" name="Distance"/>
+    <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="NewYorkCity" displayName="NewYorkCity" ref="J1:K11" totalsRowShown="0">
-  <x:autoFilter ref="J1:K11"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Atlanta" displayName="Atlanta" ref="V1:W11" totalsRowShown="0">
+  <x:autoFilter ref="V1:W11"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="City"/>
-    <x:tableColumn id="2" name="Distance" dataDxfId="1"/>
+    <x:tableColumn id="2" name="Distance" dataDxfId="2"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -950,10 +995,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J3"/>
+  <x:dimension ref="A1:J6"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="O8" sqref="O8 O8:X10"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="B14" sqref="B14"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +1006,7 @@
     <x:col min="1" max="8" width="11" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -993,7 +1038,7 @@
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0">
         <x:v>111111</x:v>
       </x:c>
@@ -1022,7 +1067,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <x:c r="A3" s="0">
         <x:v>222222</x:v>
       </x:c>
@@ -1048,6 +1093,267 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="I3" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="0">
+        <x:v>222223</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="H4" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I4" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="0">
+        <x:v>889186</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="H5" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I5" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="0">
+        <x:v>329994</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H6" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I6" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:10">
+      <x:c r="A7" s="0">
+        <x:v>960147</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="H7" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I7" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:10">
+      <x:c r="A8" s="0">
+        <x:v>823575</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H8" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I8" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:10">
+      <x:c r="A9" s="0">
+        <x:v>290666</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H9" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I9" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
+      <x:c r="A10" s="0">
+        <x:v>324477</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H10" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I10" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:10">
+      <x:c r="A11" s="0">
+        <x:v>578896</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F11" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="G11" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H11" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I11" s="0">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:10">
+      <x:c r="A12" s="0">
+        <x:v>306218</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F12" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="G12" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H12" s="0">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="I12" s="0">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -1081,35 +1387,35 @@
   <x:sheetData>
     <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F1" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D2" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <x:c r="D3" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1141,7 +1447,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
@@ -1155,7 +1461,7 @@
     </x:row>
     <x:row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -1190,16 +1496,16 @@
   <x:sheetData>
     <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>46</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1232,7 +1538,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E6"/>
+  <x:dimension ref="A1:E9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
       <x:selection activeCell="E8" sqref="E8"/>
@@ -1245,96 +1551,96 @@
   <x:sheetData>
     <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>50</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A2" s="4" t="s">
-        <x:v>33</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B2" s="5" t="s">
-        <x:v>34</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C2" s="5" t="s">
-        <x:v>35</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D2" s="6" t="s">
-        <x:v>36</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="E2" s="1"/>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="17" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="B3" s="18" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="C3" s="18" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="D3" s="19" t="s">
-        <x:v>36</x:v>
+      <x:c r="A3" s="12" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="B3" s="13" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="C3" s="13" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="D3" s="14" t="s">
+        <x:v>54</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="17" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="B4" s="18" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C4" s="18" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="D4" s="19" t="s">
-        <x:v>43</x:v>
+      <x:c r="A4" s="12" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B4" s="13" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C4" s="13" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D4" s="14" t="s">
+        <x:v>61</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="17" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="B5" s="18" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C5" s="18" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="D5" s="19" t="s">
-        <x:v>44</x:v>
+      <x:c r="A5" s="12" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B5" s="13" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C5" s="13" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D5" s="14" t="s">
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="17" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="B6" s="18" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="C6" s="18" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="D6" s="19" t="s">
-        <x:v>45</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
+      <x:c r="A6" s="12" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B6" s="13" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C6" s="13" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="D6" s="14" t="s">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="D7" s="1"/>
     </x:row>
-    <x:row r="8" spans="1:5">
+    <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="D8" s="1"/>
     </x:row>
-    <x:row r="9" spans="1:5">
+    <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="D9" s="1"/>
     </x:row>
   </x:sheetData>
@@ -1355,7 +1661,7 @@
   </x:sheetPr>
   <x:dimension ref="A1:AF13"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
+    <x:sheetView workbookViewId="0">
       <x:selection activeCell="W23" sqref="W23"/>
     </x:sheetView>
   </x:sheetViews>
@@ -1380,790 +1686,790 @@
     <x:col min="28" max="29" width="11" style="0" customWidth="1"/>
     <x:col min="30" max="30" width="9.140625" style="0" customWidth="1"/>
     <x:col min="31" max="32" width="11" style="0" customWidth="1"/>
-    <x:col min="33" max="16384" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="33" max="33" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="H1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="J1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="K1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="M1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="N1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="P1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="Q1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="S1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="T1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="V1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="W1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="Y1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="Z1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="AB1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="AC1" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="AE1" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="AF1" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="B2" s="20">
+        <x:v>65</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B2" s="10">
         <x:v>459</x:v>
       </x:c>
-      <x:c r="D2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="E2" s="13">
+      <x:c r="D2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="E2" s="9">
         <x:v>459</x:v>
       </x:c>
-      <x:c r="G2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="H2" s="13">
+      <x:c r="G2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="H2" s="9">
         <x:v>1780</x:v>
       </x:c>
-      <x:c r="J2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="K2" s="13">
+      <x:c r="J2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="K2" s="9">
         <x:v>760</x:v>
       </x:c>
-      <x:c r="M2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="N2" s="13">
+      <x:c r="M2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="N2" s="9">
         <x:v>1393</x:v>
       </x:c>
-      <x:c r="P2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="Q2" s="13">
+      <x:c r="P2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="Q2" s="9">
         <x:v>816</x:v>
       </x:c>
-      <x:c r="S2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="T2" s="13">
+      <x:c r="S2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="T2" s="9">
         <x:v>470</x:v>
       </x:c>
-      <x:c r="V2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="W2" s="13">
+      <x:c r="V2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="W2" s="9">
         <x:v>215</x:v>
       </x:c>
-      <x:c r="Y2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="Z2" s="13">
+      <x:c r="Y2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="Z2" s="9">
         <x:v>397</x:v>
       </x:c>
-      <x:c r="AB2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="AC2" s="13">
+      <x:c r="AB2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="AC2" s="9">
         <x:v>1580</x:v>
       </x:c>
-      <x:c r="AE2" s="20" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="AF2" s="13">
+      <x:c r="AE2" s="10" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="AF2" s="9">
         <x:v>567</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="B3" s="20">
+    <x:row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B3" s="10">
         <x:v>1780</x:v>
       </x:c>
-      <x:c r="D3" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="E3" s="13">
+      <x:c r="D3" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="E3" s="9">
         <x:v>2049</x:v>
       </x:c>
-      <x:c r="G3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="H3" s="13">
+      <x:c r="G3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="H3" s="9">
         <x:v>2049</x:v>
       </x:c>
-      <x:c r="J3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="K3" s="13">
+      <x:c r="J3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="K3" s="9">
         <x:v>405</x:v>
       </x:c>
-      <x:c r="M3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="N3" s="13">
+      <x:c r="M3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="N3" s="9">
         <x:v>1568</x:v>
       </x:c>
-      <x:c r="P3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="Q3" s="13">
+      <x:c r="P3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="Q3" s="9">
         <x:v>1088</x:v>
       </x:c>
-      <x:c r="S3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="T3" s="13">
+      <x:c r="S3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="T3" s="9">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="V3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="W3" s="13">
+      <x:c r="V3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="W3" s="9">
         <x:v>555</x:v>
       </x:c>
-      <x:c r="Y3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="Z3" s="13">
+      <x:c r="Y3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="Z3" s="9">
         <x:v>308</x:v>
       </x:c>
-      <x:c r="AB3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="AC3" s="13">
+      <x:c r="AB3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="AC3" s="9">
         <x:v>1830</x:v>
       </x:c>
-      <x:c r="AE3" s="20" t="s">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="AF3" s="13">
+      <x:c r="AE3" s="10" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="AF3" s="9">
         <x:v>304</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="20" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="B4" s="20">
+    <x:row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B4" s="10">
         <x:v>760</x:v>
       </x:c>
-      <x:c r="D4" s="20" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="E4" s="13">
+      <x:c r="D4" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="E4" s="9">
         <x:v>405</x:v>
       </x:c>
-      <x:c r="G4" s="20" t="s">
-        <x:v>49</x:v>
-      </x:c>
-      <x:c r="H4" s="13">
+      <x:c r="G4" s="10" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="H4" s="9">
         <x:v>2541</x:v>
       </x:c>
-      <x:c r="J4" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="K4" s="13">
+      <x:c r="J4" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="K4" s="9">
         <x:v>2541</x:v>
       </x:c>
-      <x:c r="M4" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="N4" s="13">
+      <x:c r="M4" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="N4" s="9">
         <x:v>579</x:v>
       </x:c>
-      <x:c r="P4" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="Q4" s="13">
+      <x:c r="P4" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="Q4" s="9">
         <x:v>2339</x:v>
       </x:c>
-      <x:c r="S4" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="T4" s="13">
+      <x:c r="S4" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="T4" s="9">
         <x:v>1983</x:v>
       </x:c>
-      <x:c r="V4" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="W4" s="13">
+      <x:c r="V4" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="W4" s="9">
         <x:v>1937</x:v>
       </x:c>
-      <x:c r="Y4" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="Z4" s="13">
+      <x:c r="Y4" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="Z4" s="9">
         <x:v>1746</x:v>
       </x:c>
-      <x:c r="AB4" s="20" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="AC4" s="13">
+      <x:c r="AB4" s="10" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="AC4" s="9">
         <x:v>228</x:v>
       </x:c>
-      <x:c r="AE4" s="20" t="s">
-        <x:v>48</x:v>
+      <x:c r="AE4" s="10" t="s">
+        <x:v>66</x:v>
       </x:c>
       <x:c r="AF4" s="0">
         <x:v>2299</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="B5" s="20">
+    <x:row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B5" s="10">
         <x:v>1393</x:v>
       </x:c>
-      <x:c r="D5" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="E5" s="13">
+      <x:c r="D5" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="E5" s="9">
         <x:v>1568</x:v>
       </x:c>
-      <x:c r="G5" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="H5" s="13">
+      <x:c r="G5" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="H5" s="9">
         <x:v>579</x:v>
       </x:c>
-      <x:c r="J5" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="K5" s="13">
+      <x:c r="J5" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="K5" s="9">
         <x:v>1973</x:v>
       </x:c>
-      <x:c r="M5" s="20" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="N5" s="13">
+      <x:c r="M5" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="N5" s="9">
         <x:v>1973</x:v>
       </x:c>
-      <x:c r="P5" s="20" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="Q5" s="13">
+      <x:c r="P5" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="Q5" s="9">
         <x:v>1090</x:v>
       </x:c>
-      <x:c r="S5" s="20" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="T5" s="13">
+      <x:c r="S5" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="T5" s="9">
         <x:v>482</x:v>
       </x:c>
-      <x:c r="V5" s="20" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="W5" s="13">
+      <x:c r="V5" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="W5" s="9">
         <x:v>746</x:v>
       </x:c>
-      <x:c r="Y5" s="20" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="Z5" s="13">
+      <x:c r="Y5" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="Z5" s="9">
         <x:v>713</x:v>
       </x:c>
-      <x:c r="AB5" s="20" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="AC5" s="13">
+      <x:c r="AB5" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="AC5" s="9">
         <x:v>228</x:v>
       </x:c>
-      <x:c r="AE5" s="20" t="s">
-        <x:v>51</x:v>
-      </x:c>
-      <x:c r="AF5" s="13">
+      <x:c r="AE5" s="10" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="AF5" s="9">
         <x:v>204</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="B6" s="20">
+    <x:row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A6" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="B6" s="10">
         <x:v>816</x:v>
       </x:c>
-      <x:c r="D6" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="E6" s="13">
+      <x:c r="D6" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="E6" s="9">
         <x:v>1088</x:v>
       </x:c>
-      <x:c r="G6" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="H6" s="13">
+      <x:c r="G6" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="H6" s="9">
         <x:v>2339</x:v>
       </x:c>
-      <x:c r="J6" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="K6" s="13">
+      <x:c r="J6" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="K6" s="9">
         <x:v>1090</x:v>
       </x:c>
-      <x:c r="M6" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="N6" s="13">
+      <x:c r="M6" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="N6" s="9">
         <x:v>2090</x:v>
       </x:c>
-      <x:c r="P6" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="Q6" s="13">
+      <x:c r="P6" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="Q6" s="9">
         <x:v>2090</x:v>
       </x:c>
-      <x:c r="S6" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="T6" s="13">
+      <x:c r="S6" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="T6" s="9">
         <x:v>1492</x:v>
       </x:c>
-      <x:c r="V6" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="W6" s="13">
+      <x:c r="V6" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="W6" s="9">
         <x:v>1584</x:v>
       </x:c>
-      <x:c r="Y6" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="Z6" s="13">
+      <x:c r="Y6" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="Z6" s="9">
         <x:v>1260</x:v>
       </x:c>
-      <x:c r="AB6" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="AC6" s="13">
+      <x:c r="AB6" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="AC6" s="9">
         <x:v>362</x:v>
       </x:c>
-      <x:c r="AE6" s="20" t="s">
-        <x:v>50</x:v>
-      </x:c>
-      <x:c r="AF6" s="13">
+      <x:c r="AE6" s="10" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="AF6" s="9">
         <x:v>1846</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="B7" s="20">
+    <x:row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A7" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B7" s="10">
         <x:v>470</x:v>
       </x:c>
-      <x:c r="D7" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="E7" s="13">
+      <x:c r="D7" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="E7" s="9">
         <x:v>90</x:v>
       </x:c>
-      <x:c r="G7" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="H7" s="13">
+      <x:c r="G7" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="H7" s="9">
         <x:v>1983</x:v>
       </x:c>
-      <x:c r="J7" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="K7" s="13">
+      <x:c r="J7" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="K7" s="9">
         <x:v>482</x:v>
       </x:c>
-      <x:c r="M7" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="N7" s="13">
+      <x:c r="M7" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="N7" s="9">
         <x:v>1492</x:v>
       </x:c>
-      <x:c r="P7" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="Q7" s="13">
+      <x:c r="P7" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="Q7" s="9">
         <x:v>1154</x:v>
       </x:c>
-      <x:c r="S7" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="T7" s="13">
+      <x:c r="S7" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="T7" s="9">
         <x:v>1154</x:v>
       </x:c>
-      <x:c r="V7" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="W7" s="13">
+      <x:c r="V7" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="W7" s="9">
         <x:v>605</x:v>
       </x:c>
-      <x:c r="Y7" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="Z7" s="13">
+      <x:c r="Y7" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Z7" s="9">
         <x:v>1189</x:v>
       </x:c>
-      <x:c r="AB7" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="AC7" s="13">
+      <x:c r="AB7" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AC7" s="9">
         <x:v>2181</x:v>
       </x:c>
-      <x:c r="AE7" s="20" t="s">
-        <x:v>52</x:v>
-      </x:c>
-      <x:c r="AF7" s="13">
+      <x:c r="AE7" s="10" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="AF7" s="9">
         <x:v>924</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="B8" s="20">
+    <x:row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A8" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="B8" s="10">
         <x:v>215</x:v>
       </x:c>
-      <x:c r="D8" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="E8" s="13">
+      <x:c r="D8" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E8" s="9">
         <x:v>555</x:v>
       </x:c>
-      <x:c r="G8" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="H8" s="13">
+      <x:c r="G8" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="H8" s="9">
         <x:v>1937</x:v>
       </x:c>
-      <x:c r="J8" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="K8" s="13">
+      <x:c r="J8" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="K8" s="9">
         <x:v>746</x:v>
       </x:c>
-      <x:c r="M8" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="N8" s="13">
+      <x:c r="M8" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="N8" s="9">
         <x:v>1584</x:v>
       </x:c>
-      <x:c r="P8" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="Q8" s="13">
+      <x:c r="P8" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="Q8" s="9">
         <x:v>605</x:v>
       </x:c>
-      <x:c r="S8" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="T8" s="13">
+      <x:c r="S8" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="T8" s="9">
         <x:v>596</x:v>
       </x:c>
-      <x:c r="V8" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="W8" s="13">
+      <x:c r="V8" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="W8" s="9">
         <x:v>596</x:v>
       </x:c>
-      <x:c r="Y8" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="Z8" s="13">
+      <x:c r="Y8" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="Z8" s="9">
         <x:v>283</x:v>
       </x:c>
-      <x:c r="AB8" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="AC8" s="13">
+      <x:c r="AB8" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AC8" s="9">
         <x:v>1762</x:v>
       </x:c>
-      <x:c r="AE8" s="20" t="s">
-        <x:v>53</x:v>
-      </x:c>
-      <x:c r="AF8" s="13">
+      <x:c r="AE8" s="10" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="AF8" s="9">
         <x:v>394</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="B9" s="20">
+    <x:row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B9" s="10">
         <x:v>397</x:v>
       </x:c>
-      <x:c r="D9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="E9" s="13">
+      <x:c r="D9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="E9" s="9">
         <x:v>308</x:v>
       </x:c>
-      <x:c r="G9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="H9" s="13">
+      <x:c r="G9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="H9" s="9">
         <x:v>1746</x:v>
       </x:c>
-      <x:c r="J9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="K9" s="13">
+      <x:c r="J9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="K9" s="9">
         <x:v>713</x:v>
       </x:c>
-      <x:c r="M9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="N9" s="13">
+      <x:c r="M9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="N9" s="9">
         <x:v>1260</x:v>
       </x:c>
-      <x:c r="P9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="Q9" s="13">
+      <x:c r="P9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="Q9" s="9">
         <x:v>1189</x:v>
       </x:c>
-      <x:c r="S9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="T9" s="13">
+      <x:c r="S9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="T9" s="9">
         <x:v>283</x:v>
       </x:c>
-      <x:c r="V9" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="W9" s="13">
+      <x:c r="V9" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="W9" s="9">
         <x:v>588</x:v>
       </x:c>
-      <x:c r="Y9" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="Z9" s="13">
+      <x:c r="Y9" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="Z9" s="9">
         <x:v>588</x:v>
       </x:c>
-      <x:c r="AB9" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="AC9" s="13">
+      <x:c r="AB9" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="AC9" s="9">
         <x:v>1746</x:v>
       </x:c>
-      <x:c r="AE9" s="20" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="AF9" s="13">
+      <x:c r="AE9" s="10" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="AF9" s="9">
         <x:v>543</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="B10" s="20">
+    <x:row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="B10" s="10">
         <x:v>1580</x:v>
       </x:c>
-      <x:c r="D10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="E10" s="13">
+      <x:c r="D10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="E10" s="9">
         <x:v>1830</x:v>
       </x:c>
-      <x:c r="G10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="H10" s="13">
+      <x:c r="G10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="H10" s="9">
         <x:v>228</x:v>
       </x:c>
-      <x:c r="J10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="K10" s="13">
+      <x:c r="J10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="K10" s="9">
         <x:v>2233</x:v>
       </x:c>
-      <x:c r="M10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="N10" s="13">
+      <x:c r="M10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="N10" s="9">
         <x:v>362</x:v>
       </x:c>
-      <x:c r="P10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="Q10" s="13">
+      <x:c r="P10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="Q10" s="9">
         <x:v>2181</x:v>
       </x:c>
-      <x:c r="S10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="T10" s="13">
+      <x:c r="S10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="T10" s="9">
         <x:v>1762</x:v>
       </x:c>
-      <x:c r="V10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="W10" s="13">
+      <x:c r="V10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="W10" s="9">
         <x:v>1746</x:v>
       </x:c>
-      <x:c r="Y10" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="Z10" s="13">
+      <x:c r="Y10" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="Z10" s="9">
         <x:v>1525</x:v>
       </x:c>
-      <x:c r="AB10" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="AC10" s="13">
+      <x:c r="AB10" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="AC10" s="9">
         <x:v>1525</x:v>
       </x:c>
-      <x:c r="AE10" s="20" t="s">
-        <x:v>55</x:v>
-      </x:c>
-      <x:c r="AF10" s="13">
+      <x:c r="AE10" s="10" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="AF10" s="9">
         <x:v>595</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="20" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="B11" s="20">
+    <x:row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <x:c r="A11" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="B11" s="10">
         <x:v>567</x:v>
       </x:c>
-      <x:c r="D11" s="20" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="E11" s="13">
+      <x:c r="D11" s="10" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="E11" s="9">
         <x:v>304</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="H11" s="21">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="H11" s="11">
         <x:v>2296</x:v>
       </x:c>
       <x:c r="J11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="K11" s="13">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="K11" s="9">
         <x:v>204</x:v>
       </x:c>
       <x:c r="M11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="N11" s="13">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="N11" s="9">
         <x:v>1846</x:v>
       </x:c>
       <x:c r="P11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="Q11" s="13">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Q11" s="9">
         <x:v>924</x:v>
       </x:c>
       <x:c r="S11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="T11" s="13">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="T11" s="9">
         <x:v>394</x:v>
       </x:c>
       <x:c r="V11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="W11" s="13">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="W11" s="9">
         <x:v>543</x:v>
       </x:c>
       <x:c r="Y11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="Z11" s="13">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="Z11" s="9">
         <x:v>595</x:v>
       </x:c>
       <x:c r="AB11" s="0" t="s">
-        <x:v>57</x:v>
-      </x:c>
-      <x:c r="AC11" s="13">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="AC11" s="9">
         <x:v>2086</x:v>
       </x:c>
-      <x:c r="AE11" s="20" t="s">
-        <x:v>56</x:v>
-      </x:c>
-      <x:c r="AF11" s="13">
+      <x:c r="AE11" s="10" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="AF11" s="9">
         <x:v>2086</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <x:row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A13" s="0" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="D13" s="10" t="s">
-        <x:v>42</x:v>
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="D13" s="8" t="s">
+        <x:v>60</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="J13" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="M13" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="P13" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="S13" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="V13" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="Y13" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="AB13" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="AE13" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>79</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Accounting Manager complete + load engineer changes
- Completed both functions for accounting manager
- Updated customer history when a flight is edited
</commit_message>
<xml_diff>
--- a/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
+++ b/SWE Project/SWE Project/bin/Debug/net6.0/AirportInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dxvia\Documents\GitHub\EECS-3550-Team-2\SWE Project\SWE Project\bin\Debug\net6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC8274B-96E7-496D-9D62-2F887CF155E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2692EC7C-307F-4666-92B0-D4F521C5012C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3FBE4BD0-15DC-440E-AAB6-2D33A5BF3E36}"/>
   </bookViews>
   <sheets>
     <sheet name="CustList" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="64">
   <si>
     <t>UserID</t>
   </si>
@@ -73,6 +73,9 @@
     <t>CardInfo</t>
   </si>
   <si>
+    <t>000000</t>
+  </si>
+  <si>
     <t>John</t>
   </si>
   <si>
@@ -82,12 +85,33 @@
     <t>123 Alm Street</t>
   </si>
   <si>
+    <t>000001</t>
+  </si>
+  <si>
     <t>Jane</t>
   </si>
   <si>
     <t>321 Ren Rd</t>
   </si>
   <si>
+    <t>000002</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>000003</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
     <t>CustID</t>
   </si>
   <si>
@@ -109,7 +133,19 @@
     <t>Points Used</t>
   </si>
   <si>
-    <t>booked</t>
+    <t>555</t>
+  </si>
+  <si>
+    <t>5/20/2023 12:00:00 PM</t>
+  </si>
+  <si>
+    <t>Booked</t>
+  </si>
+  <si>
+    <t>nashville</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
   </si>
   <si>
     <t>EmpID</t>
@@ -139,7 +175,7 @@
     <t>123</t>
   </si>
   <si>
-    <t>nashville</t>
+    <t>Nashville</t>
   </si>
   <si>
     <t>4/7/2023 5:50 PM</t>
@@ -148,16 +184,13 @@
     <t>456</t>
   </si>
   <si>
-    <t>555</t>
-  </si>
-  <si>
-    <t>Nashville</t>
-  </si>
-  <si>
-    <t>Cleveland</t>
-  </si>
-  <si>
-    <t>4/12/2023 9:43 PM</t>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>05/20/2023 12:00 PM</t>
   </si>
   <si>
     <t>City</t>
@@ -181,18 +214,12 @@
     <t>Miami</t>
   </si>
   <si>
-    <t>Detroit</t>
-  </si>
-  <si>
     <t>Atlanta</t>
   </si>
   <si>
     <t>Chicago</t>
   </si>
   <si>
-    <t>Las Vegas</t>
-  </si>
-  <si>
     <t>Washington DC</t>
   </si>
   <si>
@@ -206,30 +233,6 @@
   </si>
   <si>
     <t>WashingtonDc</t>
-  </si>
-  <si>
-    <t>000000</t>
-  </si>
-  <si>
-    <t>000001</t>
-  </si>
-  <si>
-    <t>000002</t>
-  </si>
-  <si>
-    <t>000003</t>
-  </si>
-  <si>
-    <t>000004</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>Jake</t>
-  </si>
-  <si>
-    <t>Justin</t>
   </si>
 </sst>
 </file>
@@ -344,7 +347,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -360,6 +363,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,6 +380,16 @@
     </dxf>
     <dxf>
       <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <sz val="10"/>
       </font>
@@ -404,16 +419,6 @@
     </dxf>
     <dxf>
       <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <sz val="10"/>
       </font>
@@ -489,16 +494,50 @@
       <font>
         <color theme="1"/>
       </font>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
         <color theme="1"/>
       </font>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
       <font>
         <color theme="1"/>
       </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -560,6 +599,7 @@
       <font>
         <color theme="1"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -594,33 +634,33 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Nashville" displayName="Nashville" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="LosAngeles" displayName="LosAngeles" ref="G1:H11" totalsRowShown="0">
+  <autoFilter ref="G1:H11" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="City" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Distance" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="City"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Distance"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="SaltLakeCity" displayName="SaltLakeCity" ref="M1:N11" totalsRowShown="0">
-  <autoFilter ref="M1:N11" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="LasVegas" displayName="LasVegas" ref="AB1:AC11" totalsRowShown="0">
+  <autoFilter ref="AB1:AC11" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="City"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Distance" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Distance" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="LasVegas" displayName="LasVegas" ref="AB1:AC11" totalsRowShown="0">
-  <autoFilter ref="AB1:AC11" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="SaltLakeCity" displayName="SaltLakeCity" ref="M1:N11" totalsRowShown="0">
+  <autoFilter ref="M1:N11" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="City"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Distance" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Distance" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -631,7 +671,7 @@
   <autoFilter ref="J1:K11" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="City"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Distance" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Distance" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -642,18 +682,18 @@
   <autoFilter ref="Y1:Z11" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="City"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Distance" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Distance" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="LosAngeles" displayName="LosAngeles" ref="G1:H11" totalsRowShown="0">
-  <autoFilter ref="G1:H11" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="Nashville" displayName="Nashville" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="City"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Distance"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="City" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Distance" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,8 +766,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Detroit" displayName="Detroit" ref="S1:T11" totalsRowShown="0">
-  <autoFilter ref="S1:T11" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Miami" displayName="Miami" ref="P1:Q11" totalsRowShown="0">
+  <autoFilter ref="P1:Q11" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="City"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Distance" dataDxfId="11"/>
@@ -748,8 +788,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Miami" displayName="Miami" ref="P1:Q11" totalsRowShown="0">
-  <autoFilter ref="P1:Q11" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Detroit" displayName="Detroit" ref="S1:T11" totalsRowShown="0">
+  <autoFilter ref="S1:T11" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="City"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Distance" dataDxfId="8"/>
@@ -1068,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F89F44-A481-4375-B1EC-C94DE9571F7E}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,19 +1151,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>111111</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2">
         <v>1112223434</v>
@@ -1140,19 +1180,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>222222</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>7778888989</v>
@@ -1169,44 +1209,53 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>333333</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <v>444444</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>55555</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1223,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FF9086-090E-4734-B9FF-8431E3318B82}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,125 +1283,125 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2">
-        <v>555</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3">
-        <v>555</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4">
-        <v>555</v>
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5">
-        <v>555</v>
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6">
-        <v>555</v>
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1378,7 +1427,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1392,7 +1441,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1421,16 +1470,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,7 +1508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EA6902-D596-40FD-BE4B-863FCFD1EB94}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1470,59 +1521,59 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1577,135 +1628,135 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="K1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="M1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="P1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="Q1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="S1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="T1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="V1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="W1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="Y1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="Z1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AB1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="AC1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="AE1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="AF1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B2" s="10">
         <v>459</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E2" s="9">
         <v>459</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H2" s="9">
         <v>1780</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K2" s="9">
         <v>760</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="N2" s="9">
         <v>1393</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="Q2" s="9">
         <v>816</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="T2" s="9">
         <v>470</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="W2" s="9">
         <v>215</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="Z2" s="9">
         <v>397</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="AC2" s="9">
         <v>1580</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="AF2" s="9">
         <v>567</v>
@@ -1713,67 +1764,67 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3" s="10">
         <v>1780</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E3" s="9">
         <v>2049</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H3" s="9">
         <v>2049</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K3" s="9">
         <v>405</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N3" s="9">
         <v>1568</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Q3" s="9">
         <v>1088</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="T3" s="9">
         <v>90</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W3" s="9">
         <v>555</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Z3" s="9">
         <v>308</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AC3" s="9">
         <v>1830</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AF3" s="9">
         <v>304</v>
@@ -1781,67 +1832,67 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B4" s="10">
         <v>760</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E4" s="9">
         <v>405</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="H4" s="9">
         <v>2541</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="K4" s="9">
         <v>2541</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="N4" s="9">
         <v>579</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="9">
         <v>2339</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="T4" s="9">
         <v>1983</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="W4" s="9">
         <v>1937</v>
       </c>
       <c r="Y4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="Z4" s="9">
         <v>1746</v>
       </c>
       <c r="AB4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AC4" s="9">
         <v>228</v>
       </c>
       <c r="AE4" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="AF4">
         <v>2299</v>
@@ -1849,67 +1900,67 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B5" s="10">
         <v>1393</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E5" s="9">
         <v>1568</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="H5" s="9">
         <v>579</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="K5" s="9">
         <v>1973</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="N5" s="9">
         <v>1973</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="Q5" s="9">
         <v>1090</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="T5" s="9">
         <v>482</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="W5" s="9">
         <v>746</v>
       </c>
       <c r="Y5" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="Z5" s="9">
         <v>713</v>
       </c>
       <c r="AB5" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AC5" s="9">
         <v>228</v>
       </c>
       <c r="AE5" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AF5" s="9">
         <v>204</v>
@@ -1917,67 +1968,67 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B6" s="10">
         <v>816</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E6" s="9">
         <v>1088</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H6" s="9">
         <v>2339</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="K6" s="9">
         <v>1090</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="N6" s="9">
         <v>2090</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="9">
         <v>2090</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="T6" s="9">
         <v>1492</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="W6" s="9">
         <v>1584</v>
       </c>
       <c r="Y6" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="Z6" s="9">
         <v>1260</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AC6" s="9">
         <v>362</v>
       </c>
       <c r="AE6" s="10" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="AF6" s="9">
         <v>1846</v>
@@ -1985,67 +2036,67 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" s="10">
         <v>470</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="9">
         <v>90</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" s="9">
         <v>1983</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K7" s="9">
         <v>482</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N7" s="9">
         <v>1492</v>
       </c>
       <c r="P7" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="9">
         <v>1154</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="T7" s="9">
         <v>1154</v>
       </c>
       <c r="V7" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="W7" s="9">
         <v>605</v>
       </c>
       <c r="Y7" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="Z7" s="9">
         <v>1189</v>
       </c>
       <c r="AB7" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="AC7" s="9">
         <v>2181</v>
       </c>
       <c r="AE7" s="10" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="AF7" s="9">
         <v>924</v>
@@ -2053,67 +2104,67 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B8" s="10">
         <v>215</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="E8" s="9">
         <v>555</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H8" s="9">
         <v>1937</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="K8" s="9">
         <v>746</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="N8" s="9">
         <v>1584</v>
       </c>
       <c r="P8" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="Q8" s="9">
         <v>605</v>
       </c>
       <c r="S8" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="T8" s="9">
         <v>596</v>
       </c>
       <c r="V8" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W8" s="9">
         <v>596</v>
       </c>
       <c r="Y8" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Z8" s="9">
         <v>283</v>
       </c>
       <c r="AB8" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC8" s="9">
         <v>1762</v>
       </c>
       <c r="AE8" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF8" s="9">
         <v>394</v>
@@ -2121,67 +2172,67 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B9" s="10">
         <v>397</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="E9" s="9">
         <v>308</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="H9" s="9">
         <v>1746</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="K9" s="9">
         <v>713</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="N9" s="9">
         <v>1260</v>
       </c>
       <c r="P9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="Q9" s="9">
         <v>1189</v>
       </c>
       <c r="S9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="T9" s="9">
         <v>283</v>
       </c>
       <c r="V9" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="W9" s="9">
         <v>588</v>
       </c>
       <c r="Y9" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="Z9" s="9">
         <v>588</v>
       </c>
       <c r="AB9" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="AC9" s="9">
         <v>1746</v>
       </c>
       <c r="AE9" s="10" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="AF9" s="9">
         <v>543</v>
@@ -2189,67 +2240,67 @@
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="10">
         <v>1580</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="9">
         <v>1830</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="9">
         <v>228</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K10" s="9">
         <v>2233</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N10" s="9">
         <v>362</v>
       </c>
       <c r="P10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q10" s="9">
         <v>2181</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T10" s="9">
         <v>1762</v>
       </c>
       <c r="V10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="W10" s="9">
         <v>1746</v>
       </c>
       <c r="Y10" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Z10" s="9">
         <v>1525</v>
       </c>
       <c r="AB10" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="AC10" s="9">
         <v>1525</v>
       </c>
       <c r="AE10" s="10" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="AF10" s="9">
         <v>595</v>
@@ -2257,67 +2308,67 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B11" s="10">
         <v>567</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E11" s="9">
         <v>304</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="H11" s="11">
         <v>2296</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="K11" s="9">
         <v>204</v>
       </c>
       <c r="M11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="N11" s="9">
         <v>1846</v>
       </c>
       <c r="P11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Q11" s="9">
         <v>924</v>
       </c>
       <c r="S11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="T11" s="9">
         <v>394</v>
       </c>
       <c r="V11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="W11" s="9">
         <v>543</v>
       </c>
       <c r="Y11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="Z11" s="9">
         <v>595</v>
       </c>
       <c r="AB11" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="AC11" s="9">
         <v>2086</v>
       </c>
       <c r="AE11" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AF11" s="9">
         <v>2086</v>
@@ -2325,37 +2376,37 @@
     </row>
     <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="J13" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="M13" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="P13" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="S13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="V13" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="Y13" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="AB13" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="AE13" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>